<commit_message>
Fixed predictor distributions. Tried to run intial model, weird errors. Will try more ways to fix them tomorrow
</commit_message>
<xml_diff>
--- a/data/Final Project Data_long.xlsx
+++ b/data/Final Project Data_long.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtywi\Dropbox\Stastistics files\R Projects\958\958 Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtywi\Dropbox\Stastistics files\R Projects\958\958-final-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBFD741-4D2C-4E1B-AD64-1EAC8083861E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EBE485-E006-4439-B14A-6469533E505E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -468,7 +468,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="I260" workbookViewId="0">
+      <selection activeCell="W42" sqref="W42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3301,9 +3301,7 @@
       <c r="R39" s="3">
         <v>1</v>
       </c>
-      <c r="S39" s="3">
-        <v>700000</v>
-      </c>
+      <c r="S39" s="3"/>
       <c r="T39" s="3">
         <v>61</v>
       </c>

</xml_diff>